<commit_message>
update low input for other language
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -502,37 +502,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.264253306388855</v>
+        <v>0.4005992174148559</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001075931811862359</v>
+        <v>0.001320958135662688</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001011732831656947</v>
+        <v>0.001321009021407713</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001036265165304628</v>
+        <v>0.001326968804419346</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001089977932104191</v>
+        <v>0.001337755631333383</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001068639909004368</v>
+        <v>0.001302259606682322</v>
       </c>
       <c r="H2" t="n">
-        <v>0.001080956305602839</v>
+        <v>0.001352520914699046</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001033933008908724</v>
+        <v>0.001346082047645809</v>
       </c>
       <c r="J2" t="n">
-        <v>0.001047913415461532</v>
+        <v>0.001412151455557218</v>
       </c>
       <c r="K2" t="n">
-        <v>0.001066632236859086</v>
+        <v>0.001257147553487829</v>
       </c>
       <c r="L2" t="n">
-        <v>0.001033006670306959</v>
+        <v>0.001342262308842844</v>
       </c>
     </row>
     <row r="3">
@@ -542,37 +542,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2301976919174194</v>
+        <v>0.3808974742889404</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0005616338273906712</v>
+        <v>0.0008128926783114609</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0005649403967615289</v>
+        <v>0.0008286314585288792</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000560997469240542</v>
+        <v>0.0007912958531968057</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0005682548829101813</v>
+        <v>0.0008144845315110768</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0005854903892877894</v>
+        <v>0.0007983409450955706</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0005646129804826324</v>
+        <v>0.0007856259000633837</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0005530982381936474</v>
+        <v>0.0007834083582089453</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0005709998258645112</v>
+        <v>0.0008038073410336496</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0005720314439602563</v>
+        <v>0.0007859933096037899</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0005671736528485113</v>
+        <v>0.0008211272202293329</v>
       </c>
     </row>
     <row r="4">
@@ -582,37 +582,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3026641130447388</v>
+        <v>0.417898154258728</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001846011209972804</v>
+        <v>0.001471196779425049</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001855914397707011</v>
+        <v>0.00155696955310292</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001877468866232749</v>
+        <v>0.001584978388589335</v>
       </c>
       <c r="F4" t="n">
-        <v>0.001835376551699672</v>
+        <v>0.001533435695976605</v>
       </c>
       <c r="G4" t="n">
-        <v>0.001904171989181636</v>
+        <v>0.001567377295840535</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001899138206305886</v>
+        <v>0.00163751538252298</v>
       </c>
       <c r="I4" t="n">
-        <v>0.001752715673793046</v>
+        <v>0.00157297970227059</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001837430574225195</v>
+        <v>0.001584232549213486</v>
       </c>
       <c r="K4" t="n">
-        <v>0.001919293053858611</v>
+        <v>0.001574076352273593</v>
       </c>
       <c r="L4" t="n">
-        <v>0.001738702156981268</v>
+        <v>0.001336944854159966</v>
       </c>
     </row>
     <row r="5">
@@ -622,37 +622,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2758747100830078</v>
+        <v>0.4308009147644043</v>
       </c>
       <c r="C5" t="n">
-        <v>0.002638930074541033</v>
+        <v>0.002252948657780053</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002741524583850361</v>
+        <v>0.002262807712881747</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002676490970763169</v>
+        <v>0.002248883448568197</v>
       </c>
       <c r="F5" t="n">
-        <v>0.002700778352918434</v>
+        <v>0.002524382782772931</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002685520499599894</v>
+        <v>0.002323144311003329</v>
       </c>
       <c r="H5" t="n">
-        <v>0.002697429617924429</v>
+        <v>0.002289112335097263</v>
       </c>
       <c r="I5" t="n">
-        <v>0.002716878551623329</v>
+        <v>0.002179765560173839</v>
       </c>
       <c r="J5" t="n">
-        <v>0.002664615483969618</v>
+        <v>0.002385833838933442</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002697040196296733</v>
+        <v>0.002366359387835497</v>
       </c>
       <c r="L5" t="n">
-        <v>0.002665166193809566</v>
+        <v>0.002241832263523009</v>
       </c>
     </row>
     <row r="6">
@@ -662,37 +662,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2147594213485718</v>
+        <v>0.417897629737854</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001453212578960437</v>
+        <v>0.002126666105398657</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001510274677325443</v>
+        <v>0.002140130586790655</v>
       </c>
       <c r="E6" t="n">
-        <v>0.001519395305697339</v>
+        <v>0.002102052456325606</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001472564234118535</v>
+        <v>0.002153638649867529</v>
       </c>
       <c r="G6" t="n">
-        <v>0.001395669945402943</v>
+        <v>0.002074342538609472</v>
       </c>
       <c r="H6" t="n">
-        <v>0.001562288476409405</v>
+        <v>0.002170020699152436</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00153092803053124</v>
+        <v>0.002040739743025629</v>
       </c>
       <c r="J6" t="n">
-        <v>0.001493336553664447</v>
+        <v>0.00206864826471851</v>
       </c>
       <c r="K6" t="n">
-        <v>0.001482495756697805</v>
+        <v>0.002178816998491375</v>
       </c>
       <c r="L6" t="n">
-        <v>0.001446868877096047</v>
+        <v>0.002135876134368063</v>
       </c>
     </row>
     <row r="7">
@@ -702,37 +702,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2497535228729248</v>
+        <v>0.4084981203079224</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001093701363260423</v>
+        <v>0.001279828602206822</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00105193980571832</v>
+        <v>0.001153567294275217</v>
       </c>
       <c r="E7" t="n">
-        <v>0.001067786731503529</v>
+        <v>0.001143830213984285</v>
       </c>
       <c r="F7" t="n">
-        <v>0.001065875896769618</v>
+        <v>0.001179879686845021</v>
       </c>
       <c r="G7" t="n">
-        <v>0.001174698799927266</v>
+        <v>0.001159751453163368</v>
       </c>
       <c r="H7" t="n">
-        <v>0.001251094378797799</v>
+        <v>0.001212034270441093</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001066986307790051</v>
+        <v>0.001161415489798839</v>
       </c>
       <c r="J7" t="n">
-        <v>0.001058620956056388</v>
+        <v>0.00130405253035293</v>
       </c>
       <c r="K7" t="n">
-        <v>0.001042785774013546</v>
+        <v>0.001146423811782224</v>
       </c>
       <c r="L7" t="n">
-        <v>0.001140740788824936</v>
+        <v>0.001125282952403194</v>
       </c>
     </row>
     <row r="8">
@@ -742,37 +742,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2477873086929321</v>
+        <v>0.405599856376648</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002275354913830912</v>
+        <v>0.003249529243700757</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00227743637405238</v>
+        <v>0.003284297887831132</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002477767182010803</v>
+        <v>0.003371746904152045</v>
       </c>
       <c r="F8" t="n">
-        <v>0.002394806045704242</v>
+        <v>0.00319969462682308</v>
       </c>
       <c r="G8" t="n">
-        <v>0.002373900695335842</v>
+        <v>0.00330318174145612</v>
       </c>
       <c r="H8" t="n">
-        <v>0.002280430630443445</v>
+        <v>0.003335976256795498</v>
       </c>
       <c r="I8" t="n">
-        <v>0.002302628760557495</v>
+        <v>0.003315626498128426</v>
       </c>
       <c r="J8" t="n">
-        <v>0.002427708718874662</v>
+        <v>0.003358440585240588</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002278294244232326</v>
+        <v>0.003226696376824837</v>
       </c>
       <c r="L8" t="n">
-        <v>0.002383946974485184</v>
+        <v>0.003277074284011234</v>
       </c>
     </row>
     <row r="9">
@@ -782,37 +782,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2372223377227783</v>
+        <v>0.4762001514434814</v>
       </c>
       <c r="C9" t="n">
-        <v>0.001799634238166504</v>
+        <v>0.00125165633386139</v>
       </c>
       <c r="D9" t="n">
-        <v>0.001834342889085722</v>
+        <v>0.001250134424462743</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00182379452398632</v>
+        <v>0.001193910336225198</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00180999446822617</v>
+        <v>0.001191805124656818</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001851879724226163</v>
+        <v>0.001289129524254861</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001898545376842728</v>
+        <v>0.001275556195854215</v>
       </c>
       <c r="I9" t="n">
-        <v>0.001840906624160123</v>
+        <v>0.001283932905510076</v>
       </c>
       <c r="J9" t="n">
-        <v>0.001785465360712353</v>
+        <v>0.001274519216080838</v>
       </c>
       <c r="K9" t="n">
-        <v>0.001895700753405171</v>
+        <v>0.001279042059222119</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001754545400136622</v>
+        <v>0.001155256269699273</v>
       </c>
     </row>
     <row r="10">
@@ -822,37 +822,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2305070638656616</v>
+        <v>0.6005000114440918</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001561674379423904</v>
+        <v>0.001209136481563874</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001578605944265773</v>
+        <v>0.001314130181354665</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001632081584177062</v>
+        <v>0.001248534698830025</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00156334422058285</v>
+        <v>0.001264445274159228</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001522989239875512</v>
+        <v>0.001217317974356636</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001543281039651519</v>
+        <v>0.001246290820410515</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001521845688921902</v>
+        <v>0.001292309754904852</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001524000020119884</v>
+        <v>0.001250219368109974</v>
       </c>
       <c r="K10" t="n">
-        <v>0.001510419308144927</v>
+        <v>0.001308115408980854</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001574635976818636</v>
+        <v>0.001281261496954926</v>
       </c>
     </row>
     <row r="11">
@@ -862,37 +862,37 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2190849304199219</v>
+        <v>0.5336955070495606</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002469235738053949</v>
+        <v>0.002468668346290015</v>
       </c>
       <c r="D11" t="n">
-        <v>0.002569607248332631</v>
+        <v>0.002222554252754692</v>
       </c>
       <c r="E11" t="n">
-        <v>0.002363643587332953</v>
+        <v>0.002225704604886531</v>
       </c>
       <c r="F11" t="n">
-        <v>0.002473192921369681</v>
+        <v>0.002181124131378287</v>
       </c>
       <c r="G11" t="n">
-        <v>0.002515709039729749</v>
+        <v>0.002268599765873369</v>
       </c>
       <c r="H11" t="n">
-        <v>0.002496230589349366</v>
+        <v>0.002181012877730144</v>
       </c>
       <c r="I11" t="n">
-        <v>0.002412891275531971</v>
+        <v>0.002223715210613278</v>
       </c>
       <c r="J11" t="n">
-        <v>0.002400768087259848</v>
+        <v>0.002325516176668982</v>
       </c>
       <c r="K11" t="n">
-        <v>0.002559820225506469</v>
+        <v>0.002243099336718333</v>
       </c>
       <c r="L11" t="n">
-        <v>0.002547351801089742</v>
+        <v>0.002228928743833568</v>
       </c>
     </row>
     <row r="12">
@@ -902,37 +902,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4071341991424561</v>
+        <v>0.7940030336380005</v>
       </c>
       <c r="C12" t="n">
-        <v>0.004049435841245201</v>
+        <v>0.004185601927836483</v>
       </c>
       <c r="D12" t="n">
-        <v>0.004209656932351165</v>
+        <v>0.004189766472421301</v>
       </c>
       <c r="E12" t="n">
-        <v>0.004217089634046742</v>
+        <v>0.004182076925445696</v>
       </c>
       <c r="F12" t="n">
-        <v>0.004101449672533007</v>
+        <v>0.004069054299174696</v>
       </c>
       <c r="G12" t="n">
-        <v>0.004157279472949251</v>
+        <v>0.00407397125679677</v>
       </c>
       <c r="H12" t="n">
-        <v>0.004140733321998593</v>
+        <v>0.004030576733359948</v>
       </c>
       <c r="I12" t="n">
-        <v>0.004071237917425434</v>
+        <v>0.004090306906925432</v>
       </c>
       <c r="J12" t="n">
-        <v>0.004137128966123417</v>
+        <v>0.004045569728254792</v>
       </c>
       <c r="K12" t="n">
-        <v>0.004300114062112364</v>
+        <v>0.004186068785094218</v>
       </c>
       <c r="L12" t="n">
-        <v>0.004154816929738756</v>
+        <v>0.004115942608012182</v>
       </c>
     </row>
     <row r="13">
@@ -942,37 +942,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3865364074707031</v>
+        <v>0.8120952844619751</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01015923683144176</v>
+        <v>0.01000306032634224</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01022597373069315</v>
+        <v>0.0103163052688899</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01028767114750175</v>
+        <v>0.01043578685244775</v>
       </c>
       <c r="F13" t="n">
-        <v>0.009839363098805818</v>
+        <v>0.009879583942401451</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01012656227460697</v>
+        <v>0.01001800520125527</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01050095499968576</v>
+        <v>0.01030271836466662</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01007342013260091</v>
+        <v>0.01017102598300534</v>
       </c>
       <c r="J13" t="n">
-        <v>0.01033971603790232</v>
+        <v>0.009883264507019308</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01023046455160234</v>
+        <v>0.009968190601036667</v>
       </c>
       <c r="L13" t="n">
-        <v>0.009929094711784221</v>
+        <v>0.009984029389184905</v>
       </c>
     </row>
     <row r="14">
@@ -982,37 +982,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3877326011657715</v>
+        <v>0.7347992420196533</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02626193168874551</v>
+        <v>0.02136031166957306</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02684544658717445</v>
+        <v>0.0212851344809992</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02695704163746655</v>
+        <v>0.02275403525180237</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02715530333536229</v>
+        <v>0.02234803122278791</v>
       </c>
       <c r="G14" t="n">
-        <v>0.02790851827416566</v>
+        <v>0.02057703333657007</v>
       </c>
       <c r="H14" t="n">
-        <v>0.02670487908944285</v>
+        <v>0.02159284802519121</v>
       </c>
       <c r="I14" t="n">
-        <v>0.02746966150514201</v>
+        <v>0.0223129417607176</v>
       </c>
       <c r="J14" t="n">
-        <v>0.02704280548352681</v>
+        <v>0.02160899580671421</v>
       </c>
       <c r="K14" t="n">
-        <v>0.02731442875441293</v>
+        <v>0.02062579388499351</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02786204747395469</v>
+        <v>0.02083602791929782</v>
       </c>
     </row>
     <row r="15">
@@ -1022,37 +1022,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3818275213241577</v>
+        <v>0.7865546464920044</v>
       </c>
       <c r="C15" t="n">
-        <v>0.00444572277798531</v>
+        <v>0.004271537037147935</v>
       </c>
       <c r="D15" t="n">
-        <v>0.004579160109535034</v>
+        <v>0.004280742400306197</v>
       </c>
       <c r="E15" t="n">
-        <v>0.00441038254614847</v>
+        <v>0.004338583193531381</v>
       </c>
       <c r="F15" t="n">
-        <v>0.004452508529743565</v>
+        <v>0.00438064702296853</v>
       </c>
       <c r="G15" t="n">
-        <v>0.004460543723970131</v>
+        <v>0.004327643786404804</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00448028192345473</v>
+        <v>0.004325506588869948</v>
       </c>
       <c r="I15" t="n">
-        <v>0.004483906518012163</v>
+        <v>0.00440625337925227</v>
       </c>
       <c r="J15" t="n">
-        <v>0.004513398300293549</v>
+        <v>0.00444534303865507</v>
       </c>
       <c r="K15" t="n">
-        <v>0.004424141297071999</v>
+        <v>0.004270667387942086</v>
       </c>
       <c r="L15" t="n">
-        <v>0.004433455257730153</v>
+        <v>0.004332895809949161</v>
       </c>
     </row>
     <row r="16">
@@ -1062,37 +1062,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3832094192504883</v>
+        <v>0.8102074146270752</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01409595902952475</v>
+        <v>0.004618469296073011</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01432168741731432</v>
+        <v>0.004647830373093443</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01419446755855262</v>
+        <v>0.00456653273051192</v>
       </c>
       <c r="F16" t="n">
-        <v>0.01446372727893268</v>
+        <v>0.004344341570878938</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01423821801390527</v>
+        <v>0.004613848714380564</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01398427493833534</v>
+        <v>0.00466304346971204</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01436424950092497</v>
+        <v>0.004558842723134495</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01450007328203405</v>
+        <v>0.004808619218078035</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01442837125514199</v>
+        <v>0.004879021308924525</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01427188864626087</v>
+        <v>0.004754877577200063</v>
       </c>
     </row>
     <row r="17">
@@ -1102,37 +1102,37 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4171929836273193</v>
+        <v>0.7850923299789428</v>
       </c>
       <c r="C17" t="n">
-        <v>0.004698020065195883</v>
+        <v>0.004992064326538115</v>
       </c>
       <c r="D17" t="n">
-        <v>0.004740672436078721</v>
+        <v>0.004980840028311524</v>
       </c>
       <c r="E17" t="n">
-        <v>0.004724349306539366</v>
+        <v>0.00499971573573274</v>
       </c>
       <c r="F17" t="n">
-        <v>0.004665570573170202</v>
+        <v>0.005215991195999728</v>
       </c>
       <c r="G17" t="n">
-        <v>0.004726440078353354</v>
+        <v>0.005073093854687782</v>
       </c>
       <c r="H17" t="n">
-        <v>0.004697769873032953</v>
+        <v>0.005182829316172838</v>
       </c>
       <c r="I17" t="n">
-        <v>0.004815005599895712</v>
+        <v>0.005141759719460598</v>
       </c>
       <c r="J17" t="n">
-        <v>0.004642600395000611</v>
+        <v>0.004948106532492654</v>
       </c>
       <c r="K17" t="n">
-        <v>0.004723780049257202</v>
+        <v>0.005016520777842575</v>
       </c>
       <c r="L17" t="n">
-        <v>0.004677585770475478</v>
+        <v>0.005128613102143277</v>
       </c>
     </row>
     <row r="18">
@@ -1142,37 +1142,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.4498791694641113</v>
+        <v>0.8730982780456543</v>
       </c>
       <c r="C18" t="n">
-        <v>0.004830073115479084</v>
+        <v>0.004956543267275845</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004607156307693551</v>
+        <v>0.004985529945743552</v>
       </c>
       <c r="E18" t="n">
-        <v>0.004594102759409946</v>
+        <v>0.00502926211444144</v>
       </c>
       <c r="F18" t="n">
-        <v>0.004577653829964454</v>
+        <v>0.005117938553345654</v>
       </c>
       <c r="G18" t="n">
-        <v>0.004705087685133849</v>
+        <v>0.005115927666948374</v>
       </c>
       <c r="H18" t="n">
-        <v>0.004729744421848154</v>
+        <v>0.005124761428858328</v>
       </c>
       <c r="I18" t="n">
-        <v>0.004901508052422556</v>
+        <v>0.005023841965105896</v>
       </c>
       <c r="J18" t="n">
-        <v>0.004652521377283492</v>
+        <v>0.005077339537051175</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00469922114327612</v>
+        <v>0.005085115260277503</v>
       </c>
       <c r="L18" t="n">
-        <v>0.004757040202750243</v>
+        <v>0.004980500200822842</v>
       </c>
     </row>
     <row r="19">
@@ -1182,37 +1182,37 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.4029181957244873</v>
+        <v>0.8243298530578613</v>
       </c>
       <c r="C19" t="n">
-        <v>0.005378825595262755</v>
+        <v>0.005772310230729902</v>
       </c>
       <c r="D19" t="n">
-        <v>0.005124028286289131</v>
+        <v>0.005637736592379171</v>
       </c>
       <c r="E19" t="n">
-        <v>0.005158258995908685</v>
+        <v>0.005485257582557691</v>
       </c>
       <c r="F19" t="n">
-        <v>0.005007652973967458</v>
+        <v>0.005611503806824038</v>
       </c>
       <c r="G19" t="n">
-        <v>0.005219296661787304</v>
+        <v>0.005612841460525942</v>
       </c>
       <c r="H19" t="n">
-        <v>0.005203894354126177</v>
+        <v>0.005478020213978634</v>
       </c>
       <c r="I19" t="n">
-        <v>0.005064806845129581</v>
+        <v>0.005598563444739828</v>
       </c>
       <c r="J19" t="n">
-        <v>0.005221137285299196</v>
+        <v>0.005851649601823191</v>
       </c>
       <c r="K19" t="n">
-        <v>0.005344745455475144</v>
+        <v>0.005693097535796539</v>
       </c>
       <c r="L19" t="n">
-        <v>0.005292848929978089</v>
+        <v>0.005649497587000418</v>
       </c>
     </row>
     <row r="20">
@@ -1222,37 +1222,37 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.4082619667053223</v>
+        <v>0.8151936292648315</v>
       </c>
       <c r="C20" t="n">
-        <v>0.007631736129928449</v>
+        <v>0.006347187922953297</v>
       </c>
       <c r="D20" t="n">
-        <v>0.007688808891698836</v>
+        <v>0.006304864123704693</v>
       </c>
       <c r="E20" t="n">
-        <v>0.007667304275511877</v>
+        <v>0.006361689468502265</v>
       </c>
       <c r="F20" t="n">
-        <v>0.007292236901452885</v>
+        <v>0.006420142191153692</v>
       </c>
       <c r="G20" t="n">
-        <v>0.007705551580611939</v>
+        <v>0.006505251338080623</v>
       </c>
       <c r="H20" t="n">
-        <v>0.007383444413039449</v>
+        <v>0.006518035271431491</v>
       </c>
       <c r="I20" t="n">
-        <v>0.007886653501972346</v>
+        <v>0.006294172610753865</v>
       </c>
       <c r="J20" t="n">
-        <v>0.007504084512228264</v>
+        <v>0.006282340010953279</v>
       </c>
       <c r="K20" t="n">
-        <v>0.007302649027841958</v>
+        <v>0.00649495248386103</v>
       </c>
       <c r="L20" t="n">
-        <v>0.007838569195226059</v>
+        <v>0.006468554580037675</v>
       </c>
     </row>
     <row r="21">
@@ -1262,37 +1262,37 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3977069854736328</v>
+        <v>0.7894061088562012</v>
       </c>
       <c r="C21" t="n">
-        <v>0.03385531025934956</v>
+        <v>0.03168630631608825</v>
       </c>
       <c r="D21" t="n">
-        <v>0.03387860614081686</v>
+        <v>0.03344207758812251</v>
       </c>
       <c r="E21" t="n">
-        <v>0.03822719422004568</v>
+        <v>0.03195337870253828</v>
       </c>
       <c r="F21" t="n">
-        <v>0.03440235191276115</v>
+        <v>0.03116239916455841</v>
       </c>
       <c r="G21" t="n">
-        <v>0.03488904115146792</v>
+        <v>0.0319043161439918</v>
       </c>
       <c r="H21" t="n">
-        <v>0.03508004291956615</v>
+        <v>0.03221712070526552</v>
       </c>
       <c r="I21" t="n">
-        <v>0.03688233568217195</v>
+        <v>0.02942796602764908</v>
       </c>
       <c r="J21" t="n">
-        <v>0.03888971069682546</v>
+        <v>0.03175787779225633</v>
       </c>
       <c r="K21" t="n">
-        <v>0.03700413361168027</v>
+        <v>0.03389639077274059</v>
       </c>
       <c r="L21" t="n">
-        <v>0.03443404874912408</v>
+        <v>0.03157012728595958</v>
       </c>
     </row>
     <row r="22">
@@ -1302,37 +1302,37 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.5558658599853515</v>
+        <v>1.127470827102661</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01175458532067121</v>
+        <v>0.01234186456488415</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01146319295054442</v>
+        <v>0.01248596281557219</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01166134137030263</v>
+        <v>0.01253389753214143</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01174180590154737</v>
+        <v>0.01257468488750612</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01164065292124814</v>
+        <v>0.01261855336331568</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01185681440932768</v>
+        <v>0.01245474438230764</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01175426048791002</v>
+        <v>0.01259208160540927</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01176947087724701</v>
+        <v>0.01229126972333557</v>
       </c>
       <c r="K22" t="n">
-        <v>0.01219037663307436</v>
+        <v>0.01247836126065589</v>
       </c>
       <c r="L22" t="n">
-        <v>0.01168493019162149</v>
+        <v>0.01239899391278986</v>
       </c>
     </row>
     <row r="23">
@@ -1342,37 +1342,37 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.5560434341430665</v>
+        <v>1.18169949054718</v>
       </c>
       <c r="C23" t="n">
-        <v>0.02656684676286638</v>
+        <v>0.03047850267852293</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02968529333978516</v>
+        <v>0.02988216934118135</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02777397066337703</v>
+        <v>0.02991858420638362</v>
       </c>
       <c r="F23" t="n">
-        <v>0.02601597522115321</v>
+        <v>0.03040694715410997</v>
       </c>
       <c r="G23" t="n">
-        <v>0.02656327054611776</v>
+        <v>0.02993780374027198</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02782721770410802</v>
+        <v>0.02945111482267758</v>
       </c>
       <c r="I23" t="n">
-        <v>0.02669578228246764</v>
+        <v>0.02999292869870784</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02619668132705463</v>
+        <v>0.03055531968877761</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0265114081193889</v>
+        <v>0.03027110734229859</v>
       </c>
       <c r="L23" t="n">
-        <v>0.02842197810156497</v>
+        <v>0.03023286216991587</v>
       </c>
     </row>
     <row r="24">
@@ -1382,37 +1382,37 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.55263831615448</v>
+        <v>1.250000429153442</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01987723201647739</v>
+        <v>0.01660363919399214</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02017550731749369</v>
+        <v>0.01704936558477824</v>
       </c>
       <c r="E24" t="n">
-        <v>0.02014473066935495</v>
+        <v>0.01759069943547807</v>
       </c>
       <c r="F24" t="n">
-        <v>0.02073190620703989</v>
+        <v>0.01750620283891834</v>
       </c>
       <c r="G24" t="n">
-        <v>0.02019724814981529</v>
+        <v>0.01775051692499207</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02017684490778942</v>
+        <v>0.01787778151099697</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01971490586602282</v>
+        <v>0.01793195224162181</v>
       </c>
       <c r="J24" t="n">
-        <v>0.02114252241651582</v>
+        <v>0.01807311700193135</v>
       </c>
       <c r="K24" t="n">
-        <v>0.02028821705057635</v>
+        <v>0.01776731972737514</v>
       </c>
       <c r="L24" t="n">
-        <v>0.02013535023269711</v>
+        <v>0.01821099749978878</v>
       </c>
     </row>
     <row r="25">
@@ -1422,37 +1422,37 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.5566629409790039</v>
+        <v>1.174298691749573</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01980217391428918</v>
+        <v>0.02166646248865655</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01906991120991219</v>
+        <v>0.02110838863522218</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01986061086535987</v>
+        <v>0.02130570467903159</v>
       </c>
       <c r="F25" t="n">
-        <v>0.01897680389099896</v>
+        <v>0.021411932439403</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0201368865627374</v>
+        <v>0.02163138901344529</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01966755434142822</v>
+        <v>0.02100448923042338</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02036812770897373</v>
+        <v>0.02105380345099334</v>
       </c>
       <c r="J25" t="n">
-        <v>0.02028380058507026</v>
+        <v>0.02179269287234122</v>
       </c>
       <c r="K25" t="n">
-        <v>0.02006298657454425</v>
+        <v>0.02177459591065107</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0202156955520236</v>
+        <v>0.02132540009867485</v>
       </c>
     </row>
     <row r="26">
@@ -1462,37 +1462,37 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.586508059501648</v>
+        <v>1.197607040405273</v>
       </c>
       <c r="C26" t="n">
-        <v>0.09009040045339461</v>
+        <v>0.04569141824913472</v>
       </c>
       <c r="D26" t="n">
-        <v>0.08884880822933156</v>
+        <v>0.04618873951606284</v>
       </c>
       <c r="E26" t="n">
-        <v>0.08829813308117211</v>
+        <v>0.04532644794647085</v>
       </c>
       <c r="F26" t="n">
-        <v>0.08831030163587569</v>
+        <v>0.04923603861578001</v>
       </c>
       <c r="G26" t="n">
-        <v>0.08796883365710434</v>
+        <v>0.04516459809834213</v>
       </c>
       <c r="H26" t="n">
-        <v>0.08894865887933714</v>
+        <v>0.04571544546890333</v>
       </c>
       <c r="I26" t="n">
-        <v>0.08841110393252175</v>
+        <v>0.04549460007944779</v>
       </c>
       <c r="J26" t="n">
-        <v>0.08848486467291442</v>
+        <v>0.04613074612109352</v>
       </c>
       <c r="K26" t="n">
-        <v>0.08861837399787903</v>
+        <v>0.04629694825308842</v>
       </c>
       <c r="L26" t="n">
-        <v>0.08763015390021485</v>
+        <v>0.04671823141133009</v>
       </c>
     </row>
     <row r="27">
@@ -1502,37 +1502,37 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.553143048286438</v>
+        <v>1.202202820777893</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01565576682638511</v>
+        <v>0.01921799104408686</v>
       </c>
       <c r="D27" t="n">
-        <v>0.01539061644999433</v>
+        <v>0.01976443012445233</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0154738505317822</v>
+        <v>0.01909697540617621</v>
       </c>
       <c r="F27" t="n">
-        <v>0.01562125344159027</v>
+        <v>0.01950519751810779</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01574139256109792</v>
+        <v>0.01951839100663226</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0151122130669135</v>
+        <v>0.01928740445810468</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01598535551795279</v>
+        <v>0.01922748727509723</v>
       </c>
       <c r="J27" t="n">
-        <v>0.01529885175810506</v>
+        <v>0.01929430672930137</v>
       </c>
       <c r="K27" t="n">
-        <v>0.01508281777111256</v>
+        <v>0.01919067341564199</v>
       </c>
       <c r="L27" t="n">
-        <v>0.01537171532646225</v>
+        <v>0.01957713435130966</v>
       </c>
     </row>
     <row r="28">
@@ -1542,37 +1542,37 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.5563250541687011</v>
+        <v>1.170996785163879</v>
       </c>
       <c r="C28" t="n">
-        <v>0.04037187688128643</v>
+        <v>0.04455844073684844</v>
       </c>
       <c r="D28" t="n">
-        <v>0.04010827470048806</v>
+        <v>0.04606211300124492</v>
       </c>
       <c r="E28" t="n">
-        <v>0.03987636676713296</v>
+        <v>0.04645533281104136</v>
       </c>
       <c r="F28" t="n">
-        <v>0.04148764272594155</v>
+        <v>0.04811056661712402</v>
       </c>
       <c r="G28" t="n">
-        <v>0.04073064472671394</v>
+        <v>0.04416640579296978</v>
       </c>
       <c r="H28" t="n">
-        <v>0.04154935399737739</v>
+        <v>0.04586129277926307</v>
       </c>
       <c r="I28" t="n">
-        <v>0.03944635124732061</v>
+        <v>0.04700584611706328</v>
       </c>
       <c r="J28" t="n">
-        <v>0.04266915621030242</v>
+        <v>0.04437456096559958</v>
       </c>
       <c r="K28" t="n">
-        <v>0.04220752776204102</v>
+        <v>0.04465310128571356</v>
       </c>
       <c r="L28" t="n">
-        <v>0.03927881891431251</v>
+        <v>0.04483832197192886</v>
       </c>
     </row>
     <row r="29">
@@ -1582,37 +1582,37 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.5945769071578979</v>
+        <v>1.214311408996582</v>
       </c>
       <c r="C29" t="n">
-        <v>0.09906143403966021</v>
+        <v>0.04326028046794334</v>
       </c>
       <c r="D29" t="n">
-        <v>0.09475674398566873</v>
+        <v>0.04556273023375484</v>
       </c>
       <c r="E29" t="n">
-        <v>0.09991233141884198</v>
+        <v>0.04391366604543515</v>
       </c>
       <c r="F29" t="n">
-        <v>0.09505442086116254</v>
+        <v>0.04548821813773554</v>
       </c>
       <c r="G29" t="n">
-        <v>0.09656168168390278</v>
+        <v>0.04426199244249743</v>
       </c>
       <c r="H29" t="n">
-        <v>0.09883678359458208</v>
+        <v>0.04268710873176098</v>
       </c>
       <c r="I29" t="n">
-        <v>0.09783050815845841</v>
+        <v>0.04387518919279817</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0945641204619959</v>
+        <v>0.04239496272652618</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0957915715620765</v>
+        <v>0.04504055083975268</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1009116372648514</v>
+        <v>0.04506401761667112</v>
       </c>
     </row>
     <row r="30">
@@ -1622,37 +1622,37 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.6246701240539551</v>
+        <v>1.196201992034912</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01488152054637136</v>
+        <v>0.01426638762328164</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01479463784851061</v>
+        <v>0.01423617637935668</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0150554668323418</v>
+        <v>0.01373236924033459</v>
       </c>
       <c r="F30" t="n">
-        <v>0.01498549215995095</v>
+        <v>0.0142791573380768</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0150734460227023</v>
+        <v>0.01400744919290509</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01476591120310189</v>
+        <v>0.01404871311779802</v>
       </c>
       <c r="I30" t="n">
-        <v>0.01529287059563346</v>
+        <v>0.01415107828897313</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01499405289367267</v>
+        <v>0.01468251130900976</v>
       </c>
       <c r="K30" t="n">
-        <v>0.01487742153362198</v>
+        <v>0.01433741856348316</v>
       </c>
       <c r="L30" t="n">
-        <v>0.01465227497604702</v>
+        <v>0.01412552627238653</v>
       </c>
     </row>
     <row r="31">
@@ -1662,37 +1662,37 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.5643649816513061</v>
+        <v>1.187900590896606</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03521381239198073</v>
+        <v>0.03715301015646057</v>
       </c>
       <c r="D31" t="n">
-        <v>0.03523715021575577</v>
+        <v>0.03556840545046341</v>
       </c>
       <c r="E31" t="n">
-        <v>0.03457570246343775</v>
+        <v>0.03661137753860001</v>
       </c>
       <c r="F31" t="n">
-        <v>0.03433043183648754</v>
+        <v>0.03432905177148659</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0361161349859432</v>
+        <v>0.03560753748899362</v>
       </c>
       <c r="H31" t="n">
-        <v>0.03360978724324785</v>
+        <v>0.03595590090628465</v>
       </c>
       <c r="I31" t="n">
-        <v>0.03422019258817351</v>
+        <v>0.03560804928918049</v>
       </c>
       <c r="J31" t="n">
-        <v>0.03343923314145852</v>
+        <v>0.03609196197416496</v>
       </c>
       <c r="K31" t="n">
-        <v>0.03524026357476553</v>
+        <v>0.03630426992602308</v>
       </c>
       <c r="L31" t="n">
-        <v>0.03366614036451217</v>
+        <v>0.03575618258881911</v>
       </c>
     </row>
     <row r="32">
@@ -1702,37 +1702,37 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.8064674615859986</v>
+        <v>1.801304984092712</v>
       </c>
       <c r="C32" t="n">
-        <v>0.105270959321238</v>
+        <v>0.1430833564868907</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1052652556402769</v>
+        <v>0.1421493508510323</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1052571437563197</v>
+        <v>0.1422206904146285</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1053321077514919</v>
+        <v>0.1427957511945326</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1052999755247371</v>
+        <v>0.1450094818214229</v>
       </c>
       <c r="H32" t="n">
-        <v>0.1052486828964198</v>
+        <v>0.1432702877173832</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1052483400012704</v>
+        <v>0.144337803128223</v>
       </c>
       <c r="J32" t="n">
-        <v>0.105245446159999</v>
+        <v>0.1402431016243171</v>
       </c>
       <c r="K32" t="n">
-        <v>0.1052601008359575</v>
+        <v>0.1445066564237798</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1053158073022073</v>
+        <v>0.1429951978252711</v>
       </c>
     </row>
     <row r="33">
@@ -1742,37 +1742,37 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.7207869768142701</v>
+        <v>1.629165315628052</v>
       </c>
       <c r="C33" t="n">
-        <v>0.02822715956469804</v>
+        <v>0.04062785471915577</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02904297397406611</v>
+        <v>0.04047162062423955</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03004195281863997</v>
+        <v>0.04008573317645279</v>
       </c>
       <c r="F33" t="n">
-        <v>0.02918492834749666</v>
+        <v>0.04073154009879833</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03011826373530267</v>
+        <v>0.04004153629644062</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0298943946954998</v>
+        <v>0.0405614834657323</v>
       </c>
       <c r="I33" t="n">
-        <v>0.02968915309766837</v>
+        <v>0.03988158950164417</v>
       </c>
       <c r="J33" t="n">
-        <v>0.02951777750717779</v>
+        <v>0.04084262611688074</v>
       </c>
       <c r="K33" t="n">
-        <v>0.02935240672421881</v>
+        <v>0.04089339599860384</v>
       </c>
       <c r="L33" t="n">
-        <v>0.02989293767668162</v>
+        <v>0.0405220705254448</v>
       </c>
     </row>
     <row r="34">
@@ -1782,37 +1782,37 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.9187126874923706</v>
+        <v>1.845098614692688</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1540497738049088</v>
+        <v>0.1447863270389388</v>
       </c>
       <c r="D34" t="n">
-        <v>0.146235454668564</v>
+        <v>0.144804437066867</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1369170809465016</v>
+        <v>0.1447903657538341</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1516896073428008</v>
+        <v>0.1447869842490297</v>
       </c>
       <c r="G34" t="n">
-        <v>0.1485514143061825</v>
+        <v>0.1447894586899907</v>
       </c>
       <c r="H34" t="n">
-        <v>0.145730610234885</v>
+        <v>0.1448003225237233</v>
       </c>
       <c r="I34" t="n">
-        <v>0.1380860612925353</v>
+        <v>0.1447864266474688</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1468321541024483</v>
+        <v>0.1447875923702562</v>
       </c>
       <c r="K34" t="n">
-        <v>0.09813070916775241</v>
+        <v>0.1447880393630139</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1480394250083104</v>
+        <v>0.1447860119863096</v>
       </c>
     </row>
     <row r="35">
@@ -1822,37 +1822,37 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.7209741353988648</v>
+        <v>1.631975150108337</v>
       </c>
       <c r="C35" t="n">
-        <v>0.03363108021727355</v>
+        <v>0.03847739628200558</v>
       </c>
       <c r="D35" t="n">
-        <v>0.03233338035141438</v>
+        <v>0.03926929975336473</v>
       </c>
       <c r="E35" t="n">
-        <v>0.03330244205933926</v>
+        <v>0.03896804524729109</v>
       </c>
       <c r="F35" t="n">
-        <v>0.03300778859018293</v>
+        <v>0.03815470759565642</v>
       </c>
       <c r="G35" t="n">
-        <v>0.03323288540780071</v>
+        <v>0.0371852667730546</v>
       </c>
       <c r="H35" t="n">
-        <v>0.03369341589002481</v>
+        <v>0.03859272633895287</v>
       </c>
       <c r="I35" t="n">
-        <v>0.03274929805929903</v>
+        <v>0.03799656516658616</v>
       </c>
       <c r="J35" t="n">
-        <v>0.03461458656938908</v>
+        <v>0.03712897776958152</v>
       </c>
       <c r="K35" t="n">
-        <v>0.03297667643889671</v>
+        <v>0.03844250598841311</v>
       </c>
       <c r="L35" t="n">
-        <v>0.03223008141481862</v>
+        <v>0.0392143599811041</v>
       </c>
     </row>
     <row r="36">
@@ -1862,37 +1862,37 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.7624124765396119</v>
+        <v>1.71910388469696</v>
       </c>
       <c r="C36" t="n">
-        <v>0.09439572562420165</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="D36" t="n">
-        <v>0.09415280731103343</v>
+        <v>0.10849024238091</v>
       </c>
       <c r="E36" t="n">
-        <v>0.09325113117515757</v>
+        <v>0.1084877935419579</v>
       </c>
       <c r="F36" t="n">
-        <v>0.09298371158264709</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="G36" t="n">
-        <v>0.09298060939411906</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="H36" t="n">
-        <v>0.09289664769073672</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="I36" t="n">
-        <v>0.09311159303366412</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="J36" t="n">
-        <v>0.09406300415960792</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="K36" t="n">
-        <v>0.09327677192739073</v>
+        <v>0.1085084843452944</v>
       </c>
       <c r="L36" t="n">
-        <v>0.09347117228492696</v>
+        <v>0.1085084843452944</v>
       </c>
     </row>
     <row r="37">
@@ -1902,37 +1902,37 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.8066970348358155</v>
+        <v>1.702096247673035</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1055467040767821</v>
+        <v>0.1486858415532454</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1448576724824094</v>
+        <v>0.1501935366335866</v>
       </c>
       <c r="E37" t="n">
-        <v>0.145166055124232</v>
+        <v>0.1485820973520763</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1436953398085115</v>
+        <v>0.1468534506504084</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1448694703860842</v>
+        <v>0.1509908425718016</v>
       </c>
       <c r="H37" t="n">
-        <v>0.144607499408174</v>
+        <v>0.1477278597584959</v>
       </c>
       <c r="I37" t="n">
-        <v>0.1447431602184983</v>
+        <v>0.1464547814625277</v>
       </c>
       <c r="J37" t="n">
-        <v>0.1457267871096131</v>
+        <v>0.1505977676752225</v>
       </c>
       <c r="K37" t="n">
-        <v>0.1441090452260549</v>
+        <v>0.1462628120725719</v>
       </c>
       <c r="L37" t="n">
-        <v>0.1440745947681833</v>
+        <v>0.1483156767365507</v>
       </c>
     </row>
     <row r="38">
@@ -1942,37 +1942,37 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.7263882160186768</v>
+        <v>1.547905731201172</v>
       </c>
       <c r="C38" t="n">
-        <v>0.03555450343932186</v>
+        <v>0.0405425673078423</v>
       </c>
       <c r="D38" t="n">
-        <v>0.03744092354825071</v>
+        <v>0.03974537364753482</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03676443864833333</v>
+        <v>0.04000340776142137</v>
       </c>
       <c r="F38" t="n">
-        <v>0.03764338875904314</v>
+        <v>0.03915718984658377</v>
       </c>
       <c r="G38" t="n">
-        <v>0.03674184631534692</v>
+        <v>0.04091253516082027</v>
       </c>
       <c r="H38" t="n">
-        <v>0.03615869363443789</v>
+        <v>0.03949378025084269</v>
       </c>
       <c r="I38" t="n">
-        <v>0.03714129575519272</v>
+        <v>0.03849284820412621</v>
       </c>
       <c r="J38" t="n">
-        <v>0.03772822863372625</v>
+        <v>0.04046135840494005</v>
       </c>
       <c r="K38" t="n">
-        <v>0.03583257805842767</v>
+        <v>0.03984620145869586</v>
       </c>
       <c r="L38" t="n">
-        <v>0.03715070719819646</v>
+        <v>0.03920423833791453</v>
       </c>
     </row>
     <row r="39">
@@ -1982,37 +1982,37 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.8463402032852173</v>
+        <v>1.612190699577332</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1294153942518461</v>
+        <v>0.1328045994308045</v>
       </c>
       <c r="D39" t="n">
-        <v>0.116178962141668</v>
+        <v>0.141306599431249</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1236419308228045</v>
+        <v>0.1388052476956204</v>
       </c>
       <c r="F39" t="n">
-        <v>0.115765605571668</v>
+        <v>0.1407773780027768</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1206250476821362</v>
+        <v>0.1329794836464191</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1258497109342643</v>
+        <v>0.1327239270090803</v>
       </c>
       <c r="I39" t="n">
-        <v>0.1164039335333932</v>
+        <v>0.1328449175956841</v>
       </c>
       <c r="J39" t="n">
-        <v>0.1165123058790381</v>
+        <v>0.1408294653939778</v>
       </c>
       <c r="K39" t="n">
-        <v>0.1236768818903444</v>
+        <v>0.1327867462046218</v>
       </c>
       <c r="L39" t="n">
-        <v>0.1129671195500059</v>
+        <v>0.1407278089611325</v>
       </c>
     </row>
     <row r="40">
@@ -2022,37 +2022,37 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.7485875606536865</v>
+        <v>1.641503858566284</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1119448212796044</v>
+        <v>0.06038844600943827</v>
       </c>
       <c r="D40" t="n">
-        <v>0.04452003632888327</v>
+        <v>0.06291120557078693</v>
       </c>
       <c r="E40" t="n">
-        <v>0.04601870691400484</v>
+        <v>0.07102861030798002</v>
       </c>
       <c r="F40" t="n">
-        <v>0.04292643833325019</v>
+        <v>0.05929075156047191</v>
       </c>
       <c r="G40" t="n">
-        <v>0.04363455347847947</v>
+        <v>0.05589238705595235</v>
       </c>
       <c r="H40" t="n">
-        <v>0.04527392437702046</v>
+        <v>0.05649149438992335</v>
       </c>
       <c r="I40" t="n">
-        <v>0.04681967777574641</v>
+        <v>0.05730428078164616</v>
       </c>
       <c r="J40" t="n">
-        <v>0.04450378513452116</v>
+        <v>0.06047197099306778</v>
       </c>
       <c r="K40" t="n">
-        <v>0.04502973409649763</v>
+        <v>0.05872780958551475</v>
       </c>
       <c r="L40" t="n">
-        <v>0.04614675068803277</v>
+        <v>0.05712312317647104</v>
       </c>
     </row>
     <row r="41">
@@ -2062,37 +2062,37 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.7884341716766358</v>
+        <v>1.608199262619018</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1103701171385202</v>
+        <v>0.1223313797082045</v>
       </c>
       <c r="D41" t="n">
-        <v>0.1101430718268682</v>
+        <v>0.1223264046107718</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1113923356633656</v>
+        <v>0.1223407468463431</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1111804484002361</v>
+        <v>0.1224947663563898</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1113911192858524</v>
+        <v>0.1223503888416799</v>
       </c>
       <c r="H41" t="n">
-        <v>0.1109633033061755</v>
+        <v>0.1225854391637083</v>
       </c>
       <c r="I41" t="n">
-        <v>0.1097624084965697</v>
+        <v>0.1223290275859035</v>
       </c>
       <c r="J41" t="n">
-        <v>0.1122228825357868</v>
+        <v>0.1223346430519035</v>
       </c>
       <c r="K41" t="n">
-        <v>0.110303554093109</v>
+        <v>0.1223284478055513</v>
       </c>
       <c r="L41" t="n">
-        <v>0.1600482408675014</v>
+        <v>0.1223262927420854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>